<commit_message>
Implemented rudimentary printers. Require more specification to tweak requirements.
</commit_message>
<xml_diff>
--- a/time-labor/week-of-22august2016.xlsx
+++ b/time-labor/week-of-22august2016.xlsx
@@ -61,6 +61,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -72,7 +73,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t xml:space="preserve">Weekly Time Record</t>
   </si>
@@ -164,7 +165,13 @@
     <t xml:space="preserve">Thursday</t>
   </si>
   <si>
+    <t xml:space="preserve">1-4, 7-9</t>
+  </si>
+  <si>
     <t xml:space="preserve">Friday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10-11, </t>
   </si>
   <si>
     <t xml:space="preserve">Saturday</t>
@@ -639,20 +646,20 @@
   <dimension ref="B1:L27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.6581632653061"/>
     <col collapsed="false" hidden="false" max="5" min="3" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.1479591836735"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -947,13 +954,17 @@
       <c r="B16" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="0"/>
+      <c r="C16" s="19" t="n">
+        <v>0.541666666666667</v>
+      </c>
+      <c r="D16" s="20" t="n">
+        <v>0.75</v>
+      </c>
       <c r="E16" s="19"/>
       <c r="F16" s="20"/>
       <c r="G16" s="21" t="n">
         <f aca="false">IF((((D16-C16)+(F16-E16))*24)&gt;8,8,((D16-C16)+(F16-E16))*24)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="H16" s="21" t="n">
         <f aca="false">IF(((D16-C16)+(F16-E16))*24&gt;8,((D16-C16)+(F16-E16))*24-8,0)</f>
@@ -962,11 +973,13 @@
       <c r="I16" s="22"/>
       <c r="J16" s="23"/>
       <c r="K16" s="24"/>
-      <c r="L16" s="0"/>
+      <c r="L16" s="0" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B17" s="18" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C17" s="19"/>
       <c r="D17" s="20"/>
@@ -983,11 +996,13 @@
       <c r="I17" s="22"/>
       <c r="J17" s="23"/>
       <c r="K17" s="24"/>
-      <c r="L17" s="0"/>
+      <c r="L17" s="0" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="18" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C18" s="19"/>
       <c r="D18" s="20"/>
@@ -1008,7 +1023,7 @@
     </row>
     <row r="19" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="18" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C19" s="19"/>
       <c r="D19" s="20"/>
@@ -1033,11 +1048,11 @@
       <c r="D20" s="25"/>
       <c r="E20" s="25"/>
       <c r="F20" s="18" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G20" s="21" t="n">
         <f aca="false">SUM(G13:G19)</f>
-        <v>9.99999999999998</v>
+        <v>15</v>
       </c>
       <c r="H20" s="21" t="n">
         <f aca="false">SUM(H13:H19)</f>
@@ -1060,7 +1075,7 @@
       <c r="D21" s="26"/>
       <c r="E21" s="25"/>
       <c r="F21" s="18" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="G21" s="28" t="n">
         <v>10</v>
@@ -1083,7 +1098,7 @@
       </c>
       <c r="G22" s="30" t="n">
         <f aca="false">G20*G21</f>
-        <v>99.9999999999998</v>
+        <v>150</v>
       </c>
       <c r="H22" s="30" t="n">
         <f aca="false">H20*H21</f>
@@ -1099,7 +1114,7 @@
       </c>
       <c r="K22" s="30" t="n">
         <f aca="false">SUM(G22:J22)</f>
-        <v>99.9999999999998</v>
+        <v>150</v>
       </c>
       <c r="L22" s="0"/>
     </row>
@@ -1130,14 +1145,14 @@
     </row>
     <row r="25" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F25" s="33" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G25" s="34"/>
       <c r="H25" s="34"/>
       <c r="I25" s="34"/>
       <c r="J25" s="34"/>
       <c r="K25" s="35" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1150,14 +1165,14 @@
     </row>
     <row r="27" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F27" s="33" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G27" s="34"/>
       <c r="H27" s="34"/>
       <c r="I27" s="34"/>
       <c r="J27" s="34"/>
       <c r="K27" s="35" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1187,7 +1202,7 @@
     <mergeCell ref="F26:I26"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation allowBlank="true" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." errorTitle="Invalid Entry" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C13:F15 C16:C19 E16:F16 D17:F19" type="time">
+    <dataValidation allowBlank="true" error="Please enter time in military time format between 0:00 and 23:59 (1:00, 8:00, 13:00, 20:00, etc.)." errorTitle="Invalid Entry" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C13:F19" type="time">
       <formula1>0</formula1>
       <formula2>0.999305555555556</formula2>
     </dataValidation>

</xml_diff>

<commit_message>
Implemented changes in specification after weekly research meeting. Documentation in research journal
</commit_message>
<xml_diff>
--- a/time-labor/week-of-22august2016.xlsx
+++ b/time-labor/week-of-22august2016.xlsx
@@ -62,6 +62,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -73,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="39">
   <si>
     <t xml:space="preserve">Weekly Time Record</t>
   </si>
@@ -169,9 +170,6 @@
   </si>
   <si>
     <t xml:space="preserve">Friday</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10-11, </t>
   </si>
   <si>
     <t xml:space="preserve">Saturday</t>
@@ -646,20 +644,20 @@
   <dimension ref="B1:L27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I17" activeCellId="0" sqref="I17"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.5255102040816"/>
     <col collapsed="false" hidden="false" max="5" min="3" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="11.8775510204082"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -981,13 +979,17 @@
       <c r="B17" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20"/>
+      <c r="C17" s="19" t="n">
+        <v>0.416666666666667</v>
+      </c>
+      <c r="D17" s="20" t="n">
+        <v>0.583333333333333</v>
+      </c>
       <c r="E17" s="19"/>
       <c r="F17" s="20"/>
       <c r="G17" s="21" t="n">
         <f aca="false">IF((((D17-C17)+(F17-E17))*24)&gt;8,8,((D17-C17)+(F17-E17))*24)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H17" s="21" t="n">
         <f aca="false">IF(((D17-C17)+(F17-E17))*24&gt;8,((D17-C17)+(F17-E17))*24-8,0)</f>
@@ -996,13 +998,11 @@
       <c r="I17" s="22"/>
       <c r="J17" s="23"/>
       <c r="K17" s="24"/>
-      <c r="L17" s="0" t="s">
-        <v>32</v>
-      </c>
+      <c r="L17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C18" s="19"/>
       <c r="D18" s="20"/>
@@ -1023,7 +1023,7 @@
     </row>
     <row r="19" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C19" s="19"/>
       <c r="D19" s="20"/>
@@ -1048,11 +1048,11 @@
       <c r="D20" s="25"/>
       <c r="E20" s="25"/>
       <c r="F20" s="18" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G20" s="21" t="n">
         <f aca="false">SUM(G13:G19)</f>
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="H20" s="21" t="n">
         <f aca="false">SUM(H13:H19)</f>
@@ -1075,7 +1075,7 @@
       <c r="D21" s="26"/>
       <c r="E21" s="25"/>
       <c r="F21" s="18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G21" s="28" t="n">
         <v>10</v>
@@ -1098,7 +1098,7 @@
       </c>
       <c r="G22" s="30" t="n">
         <f aca="false">G20*G21</f>
-        <v>150</v>
+        <v>190</v>
       </c>
       <c r="H22" s="30" t="n">
         <f aca="false">H20*H21</f>
@@ -1114,7 +1114,7 @@
       </c>
       <c r="K22" s="30" t="n">
         <f aca="false">SUM(G22:J22)</f>
-        <v>150</v>
+        <v>190</v>
       </c>
       <c r="L22" s="0"/>
     </row>
@@ -1145,14 +1145,14 @@
     </row>
     <row r="25" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F25" s="33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G25" s="34"/>
       <c r="H25" s="34"/>
       <c r="I25" s="34"/>
       <c r="J25" s="34"/>
       <c r="K25" s="35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1165,14 +1165,14 @@
     </row>
     <row r="27" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F27" s="33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G27" s="34"/>
       <c r="H27" s="34"/>
       <c r="I27" s="34"/>
       <c r="J27" s="34"/>
       <c r="K27" s="35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added lookup functions for Queue, help functionality.
</commit_message>
<xml_diff>
--- a/time-labor/week-of-22august2016.xlsx
+++ b/time-labor/week-of-22august2016.xlsx
@@ -63,6 +63,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Weekly Time Record'!$A$1:$K$27</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -644,20 +645,20 @@
   <dimension ref="B1:L27"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+      <selection pane="topLeft" activeCell="AA2" activeCellId="0" sqref="AA2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="1" width="1.08163265306122"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="15.3877551020408"/>
     <col collapsed="false" hidden="false" max="5" min="3" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="11.6071428571429"/>
     <col collapsed="false" hidden="false" max="1025" min="12" style="1" width="6.0765306122449"/>
   </cols>
   <sheetData>
@@ -1004,13 +1005,17 @@
       <c r="B18" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="20"/>
+      <c r="C18" s="19" t="n">
+        <v>0.916666666666667</v>
+      </c>
+      <c r="D18" s="20" t="n">
+        <v>0.958333333333333</v>
+      </c>
       <c r="E18" s="19"/>
       <c r="F18" s="20"/>
       <c r="G18" s="21" t="n">
         <f aca="false">IF((((D18-C18)+(F18-E18))*24)&gt;8,8,((D18-C18)+(F18-E18))*24)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" s="21" t="n">
         <f aca="false">IF(((D18-C18)+(F18-E18))*24&gt;8,((D18-C18)+(F18-E18))*24-8,0)</f>
@@ -1052,7 +1057,7 @@
       </c>
       <c r="G20" s="21" t="n">
         <f aca="false">SUM(G13:G19)</f>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H20" s="21" t="n">
         <f aca="false">SUM(H13:H19)</f>
@@ -1098,7 +1103,7 @@
       </c>
       <c r="G22" s="30" t="n">
         <f aca="false">G20*G21</f>
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="H22" s="30" t="n">
         <f aca="false">H20*H21</f>
@@ -1114,7 +1119,7 @@
       </c>
       <c r="K22" s="30" t="n">
         <f aca="false">SUM(G22:J22)</f>
-        <v>190</v>
+        <v>200</v>
       </c>
       <c r="L22" s="0"/>
     </row>

</xml_diff>